<commit_message>
Complete data and create chart
</commit_message>
<xml_diff>
--- a/data/public_laws/public_law_word_count_by_congress.xlsx
+++ b/data/public_laws/public_law_word_count_by_congress.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box Sync\GWRSC\Programming\Python\public_laws\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiezd\Documents\GitHub\Reg-Stats\data\public_laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A41BAB08-BFF9-421B-9174-6E1AC2AED19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{44D6E40E-BFC2-44A3-ADEB-B9B6898BED05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4840" yWindow="50" windowWidth="20710" windowHeight="13290" xr2:uid="{70D4D556-AEA2-45F3-AC3B-442DA83E601D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{52332C95-0FC0-4037-9150-544FEA9B962C}"/>
   </bookViews>
   <sheets>
     <sheet name="public_law_word_count_by_congre" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -31,7 +32,7 @@
     <t>Word Count</t>
   </si>
   <si>
-    <t>Law Count</t>
+    <t>Public Law Count</t>
   </si>
 </sst>
 </file>
@@ -515,9 +516,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -565,6 +565,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFA89968"/>
+      <color rgb="FF003B5C"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -597,25 +603,33 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Public Law Word Count by Congress</a:t>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>Public Law Word and Page Count by Congress</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20720566293294848"/>
+          <c:y val="1.4151625192376142E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -629,14 +643,14 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -647,7 +661,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.2965282861533832E-2"/>
+          <c:y val="9.9061376346632993E-2"/>
+          <c:w val="0.84987257615937906"/>
+          <c:h val="0.61878211973198194"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -668,7 +692,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="003B5C"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -764,79 +788,79 @@
             <c:numRef>
               <c:f>public_law_word_count_by_congre!$C$2:$C$26</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>1939610</c:v>
+                  <c:v>1959512</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2554167</c:v>
+                  <c:v>2569363</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2295760</c:v>
+                  <c:v>2323495</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1972898</c:v>
+                  <c:v>1981567</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2173388</c:v>
+                  <c:v>2177841</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3082932</c:v>
+                  <c:v>3086566</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3506546</c:v>
+                  <c:v>3508982</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3612586</c:v>
+                  <c:v>3633563</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3222478</c:v>
+                  <c:v>3222727</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3245936</c:v>
+                  <c:v>3246303</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2696475</c:v>
+                  <c:v>2700359</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3006871</c:v>
+                  <c:v>3008872</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3093894</c:v>
+                  <c:v>3110331</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2418022</c:v>
+                  <c:v>2425101</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2925809</c:v>
+                  <c:v>2926597</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3051662</c:v>
+                  <c:v>3052965</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3421269</c:v>
+                  <c:v>3423333</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3644512</c:v>
+                  <c:v>3650873</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1951861</c:v>
+                  <c:v>1973775</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2385669</c:v>
+                  <c:v>2386392</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2739320</c:v>
+                  <c:v>2739807</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3431938</c:v>
+                  <c:v>3432663</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3823226</c:v>
+                  <c:v>3826308</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3945962</c:v>
+                  <c:v>3947312</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>1628710</c:v>
@@ -846,7 +870,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EAE4-406A-8BF0-9F5B2C9D58C9}"/>
+              <c16:uniqueId val="{00000000-B3CC-442A-B10F-CC1EFD95C845}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -860,11 +884,144 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-27"/>
-        <c:axId val="1677058080"/>
-        <c:axId val="1677069600"/>
+        <c:axId val="65003824"/>
+        <c:axId val="65000464"/>
       </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>public_law_word_count_by_congre!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Page Count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="A89968"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>public_law_word_count_by_congre!$B$2:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>4118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5297</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4929</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4866</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6790</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7836</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8206</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7468</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7540</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6476</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7365</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7456</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5657</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7416</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7771</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8097</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4475</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5334</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6248</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7994</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8498</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8806</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3738</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B3CC-442A-B10F-CC1EFD95C845}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="174657936"/>
+        <c:axId val="65000944"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="1677058080"/>
+        <c:axId val="65003824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -877,20 +1034,20 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Congress</a:t>
                 </a:r>
               </a:p>
@@ -909,14 +1066,14 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -943,18 +1100,18 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-1800000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-3900000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -962,15 +1119,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1677069600"/>
+        <c:crossAx val="65000464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1677069600"/>
+        <c:axId val="65000464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -997,21 +1155,21 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Number of Words</a:t>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Thousands of words</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1029,14 +1187,14 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -1045,7 +1203,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0," sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1061,14 +1219,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -1076,10 +1234,127 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1677058080"/>
+        <c:crossAx val="65003824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="65000944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="12000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Thousands of pages</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0," sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="174657936"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="2000"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="174657936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="65000944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1088,6 +1363,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.33964750264740085"/>
+          <c:y val="0.8223463235383075"/>
+          <c:w val="0.32363693197466892"/>
+          <c:h val="3.4115763796163108E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1104,12 +1420,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1119,396 +1430,18 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>public_law_word_count_by_congre!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Page Count</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>public_law_word_count_by_congre!$B$2:$B$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>4075</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5262</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4867</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4312</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4853</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6780</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8155</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7467</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7538</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6465</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7356</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7411</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5638</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6993</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7410</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>7763</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8079</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4387</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5331</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6246</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>7991</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>8486</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>8801</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3738</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0037-48B8-8CC4-8EE148CE40D6}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="2036220672"/>
-        <c:axId val="2036219712"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2036220672"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2036219712"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2036219712"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2036220672"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2051,534 +1984,35 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{2525FBCB-916B-45D3-A8F3-03FAA89A14E1}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8654143" cy="6277429"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{622DA8C3-2D65-9EA2-B239-43B65CF9F5BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AC4B008-88AC-C13B-95B1-5A96215962D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2591,44 +2025,126 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>368299</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
-          <a:extLst>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.0108</cdr:x>
+      <cdr:y>0.87547</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.25886</cdr:x>
+      <cdr:y>0.9872</cdr:y>
+    </cdr:to>
+    <cdr:pic>
+      <cdr:nvPicPr>
+        <cdr:cNvPr id="3" name="Picture 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F830C0EA-66C9-2340-5394-A180FBB7895F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48F983BC-A634-4B33-7137-45999D4596A9}"/>
             </a:ext>
           </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+        </cdr:cNvPr>
+        <cdr:cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cdr:cNvPicPr>
+      </cdr:nvPicPr>
+      <cdr:blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </cdr:blipFill>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="93585" y="5499646"/>
+          <a:ext cx="2149010" cy="701938"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+    </cdr:pic>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.63246</cdr:x>
+      <cdr:y>0.8852</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.98429</cdr:x>
+      <cdr:y>0.97906</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF2227BD-8A17-39D7-8425-EAD580E026EF}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5479143" y="5560785"/>
+          <a:ext cx="3048000" cy="589643"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200">
+              <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Source:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0">
+              <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> Congress.gov</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="r"/>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200" baseline="0">
+            <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0">
+              <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Updated: May 20, 2025</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200">
+            <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2947,17 +2463,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B28384-0C4D-4D8D-B44A-DC42398B5807}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7771C4D6-60D8-4EA9-9AF8-72D47CBB3252}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2966,7 +2479,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -2978,10 +2491,10 @@
         <v>94</v>
       </c>
       <c r="B2">
-        <v>4075</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1939610</v>
+        <v>4118</v>
+      </c>
+      <c r="C2">
+        <v>1959512</v>
       </c>
       <c r="D2">
         <v>587</v>
@@ -2992,10 +2505,10 @@
         <v>95</v>
       </c>
       <c r="B3">
-        <v>5262</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2554167</v>
+        <v>5297</v>
+      </c>
+      <c r="C3">
+        <v>2569363</v>
       </c>
       <c r="D3">
         <v>621</v>
@@ -3006,10 +2519,10 @@
         <v>96</v>
       </c>
       <c r="B4">
-        <v>4867</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2295760</v>
+        <v>4929</v>
+      </c>
+      <c r="C4">
+        <v>2323495</v>
       </c>
       <c r="D4">
         <v>608</v>
@@ -3020,10 +2533,10 @@
         <v>97</v>
       </c>
       <c r="B5">
-        <v>4312</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1972898</v>
+        <v>4334</v>
+      </c>
+      <c r="C5">
+        <v>1981567</v>
       </c>
       <c r="D5">
         <v>469</v>
@@ -3034,10 +2547,10 @@
         <v>98</v>
       </c>
       <c r="B6">
-        <v>4853</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2173388</v>
+        <v>4866</v>
+      </c>
+      <c r="C6">
+        <v>2177841</v>
       </c>
       <c r="D6">
         <v>616</v>
@@ -3048,10 +2561,10 @@
         <v>99</v>
       </c>
       <c r="B7">
-        <v>6780</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3082932</v>
+        <v>6790</v>
+      </c>
+      <c r="C7">
+        <v>3086566</v>
       </c>
       <c r="D7">
         <v>654</v>
@@ -3062,10 +2575,10 @@
         <v>100</v>
       </c>
       <c r="B8">
-        <v>7827</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3506546</v>
+        <v>7836</v>
+      </c>
+      <c r="C8">
+        <v>3508982</v>
       </c>
       <c r="D8">
         <v>702</v>
@@ -3076,10 +2589,10 @@
         <v>101</v>
       </c>
       <c r="B9">
-        <v>8155</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3612586</v>
+        <v>8206</v>
+      </c>
+      <c r="C9">
+        <v>3633563</v>
       </c>
       <c r="D9">
         <v>640</v>
@@ -3090,10 +2603,10 @@
         <v>102</v>
       </c>
       <c r="B10">
-        <v>7467</v>
-      </c>
-      <c r="C10" s="1">
-        <v>3222478</v>
+        <v>7468</v>
+      </c>
+      <c r="C10">
+        <v>3222727</v>
       </c>
       <c r="D10">
         <v>578</v>
@@ -3104,10 +2617,10 @@
         <v>103</v>
       </c>
       <c r="B11">
-        <v>7538</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3245936</v>
+        <v>7540</v>
+      </c>
+      <c r="C11">
+        <v>3246303</v>
       </c>
       <c r="D11">
         <v>462</v>
@@ -3118,10 +2631,10 @@
         <v>104</v>
       </c>
       <c r="B12">
-        <v>6465</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2696475</v>
+        <v>6476</v>
+      </c>
+      <c r="C12">
+        <v>2700359</v>
       </c>
       <c r="D12">
         <v>333</v>
@@ -3132,10 +2645,10 @@
         <v>105</v>
       </c>
       <c r="B13">
-        <v>7356</v>
-      </c>
-      <c r="C13" s="1">
-        <v>3006871</v>
+        <v>7365</v>
+      </c>
+      <c r="C13">
+        <v>3008872</v>
       </c>
       <c r="D13">
         <v>394</v>
@@ -3146,10 +2659,10 @@
         <v>106</v>
       </c>
       <c r="B14">
-        <v>7411</v>
-      </c>
-      <c r="C14" s="1">
-        <v>3093894</v>
+        <v>7456</v>
+      </c>
+      <c r="C14">
+        <v>3110331</v>
       </c>
       <c r="D14">
         <v>580</v>
@@ -3160,10 +2673,10 @@
         <v>107</v>
       </c>
       <c r="B15">
-        <v>5638</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2418022</v>
+        <v>5657</v>
+      </c>
+      <c r="C15">
+        <v>2425101</v>
       </c>
       <c r="D15">
         <v>377</v>
@@ -3174,10 +2687,10 @@
         <v>108</v>
       </c>
       <c r="B16">
-        <v>6993</v>
-      </c>
-      <c r="C16" s="1">
-        <v>2925809</v>
+        <v>7028</v>
+      </c>
+      <c r="C16">
+        <v>2926597</v>
       </c>
       <c r="D16">
         <v>498</v>
@@ -3188,10 +2701,10 @@
         <v>109</v>
       </c>
       <c r="B17">
-        <v>7410</v>
-      </c>
-      <c r="C17" s="1">
-        <v>3051662</v>
+        <v>7416</v>
+      </c>
+      <c r="C17">
+        <v>3052965</v>
       </c>
       <c r="D17">
         <v>482</v>
@@ -3202,10 +2715,10 @@
         <v>110</v>
       </c>
       <c r="B18">
-        <v>7763</v>
-      </c>
-      <c r="C18" s="1">
-        <v>3421269</v>
+        <v>7771</v>
+      </c>
+      <c r="C18">
+        <v>3423333</v>
       </c>
       <c r="D18">
         <v>460</v>
@@ -3216,10 +2729,10 @@
         <v>111</v>
       </c>
       <c r="B19">
-        <v>8079</v>
-      </c>
-      <c r="C19" s="1">
-        <v>3644512</v>
+        <v>8097</v>
+      </c>
+      <c r="C19">
+        <v>3650873</v>
       </c>
       <c r="D19">
         <v>383</v>
@@ -3230,10 +2743,10 @@
         <v>112</v>
       </c>
       <c r="B20">
-        <v>4387</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1951861</v>
+        <v>4475</v>
+      </c>
+      <c r="C20">
+        <v>1973775</v>
       </c>
       <c r="D20">
         <v>283</v>
@@ -3244,10 +2757,10 @@
         <v>113</v>
       </c>
       <c r="B21">
-        <v>5331</v>
-      </c>
-      <c r="C21" s="1">
-        <v>2385669</v>
+        <v>5334</v>
+      </c>
+      <c r="C21">
+        <v>2386392</v>
       </c>
       <c r="D21">
         <v>292</v>
@@ -3258,10 +2771,10 @@
         <v>114</v>
       </c>
       <c r="B22">
-        <v>6246</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2739320</v>
+        <v>6248</v>
+      </c>
+      <c r="C22">
+        <v>2739807</v>
       </c>
       <c r="D22">
         <v>329</v>
@@ -3272,10 +2785,10 @@
         <v>115</v>
       </c>
       <c r="B23">
-        <v>7991</v>
-      </c>
-      <c r="C23" s="1">
-        <v>3431938</v>
+        <v>7994</v>
+      </c>
+      <c r="C23">
+        <v>3432663</v>
       </c>
       <c r="D23">
         <v>442</v>
@@ -3286,10 +2799,10 @@
         <v>116</v>
       </c>
       <c r="B24">
-        <v>8486</v>
-      </c>
-      <c r="C24" s="1">
-        <v>3823226</v>
+        <v>8498</v>
+      </c>
+      <c r="C24">
+        <v>3826308</v>
       </c>
       <c r="D24">
         <v>342</v>
@@ -3300,10 +2813,10 @@
         <v>117</v>
       </c>
       <c r="B25">
-        <v>8801</v>
-      </c>
-      <c r="C25" s="1">
-        <v>3945962</v>
+        <v>8806</v>
+      </c>
+      <c r="C25">
+        <v>3947312</v>
       </c>
       <c r="D25">
         <v>359</v>
@@ -3316,7 +2829,7 @@
       <c r="B26">
         <v>3738</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
         <v>1628710</v>
       </c>
       <c r="D26">
@@ -3330,7 +2843,7 @@
       <c r="B27">
         <v>46</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>18842</v>
       </c>
       <c r="D27">
@@ -3339,7 +2852,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Complete public law data collection and optimize code
</commit_message>
<xml_diff>
--- a/data/public_laws/public_law_word_count_by_congress.xlsx
+++ b/data/public_laws/public_law_word_count_by_congress.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxie\Documents\GitHub\Reg-Stats\data\public_laws\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiezd\Documents\GitHub\Reg-Stats\data\public_laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448BA03E-5143-4C59-88E6-0597CAB30964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="13905" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="public_law_word_count_by_congre" sheetId="1" r:id="rId1"/>
@@ -38,8 +39,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -791,34 +792,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>1959512</c:v>
+                  <c:v>1959666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2569363</c:v>
+                  <c:v>2615715</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2323495</c:v>
+                  <c:v>2331477</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1981567</c:v>
+                  <c:v>1982634</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2177841</c:v>
+                  <c:v>2187411</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3086566</c:v>
+                  <c:v>3282060</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3508982</c:v>
+                  <c:v>3513194</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3633563</c:v>
+                  <c:v>3670798</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3222727</c:v>
+                  <c:v>3249657</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3246303</c:v>
+                  <c:v>3248009</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2700359</c:v>
@@ -848,7 +849,7 @@
                   <c:v>1973775</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2386392</c:v>
+                  <c:v>2388640</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>2739807</c:v>
@@ -857,13 +858,13 @@
                   <c:v>3432663</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3826308</c:v>
+                  <c:v>3827126</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3947312</c:v>
+                  <c:v>3947924</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1628710</c:v>
+                  <c:v>1941440</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -923,34 +924,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>4118</c:v>
+                  <c:v>4119</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5297</c:v>
+                  <c:v>5403</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4929</c:v>
+                  <c:v>4948</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4334</c:v>
+                  <c:v>4339</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4866</c:v>
+                  <c:v>4889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6790</c:v>
+                  <c:v>7205</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7836</c:v>
+                  <c:v>7851</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8206</c:v>
+                  <c:v>8287</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7468</c:v>
+                  <c:v>7540</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7540</c:v>
+                  <c:v>7547</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>6476</c:v>
@@ -980,7 +981,7 @@
                   <c:v>4475</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5334</c:v>
+                  <c:v>5342</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>6248</c:v>
@@ -989,13 +990,13 @@
                   <c:v>7994</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8498</c:v>
+                  <c:v>8501</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8806</c:v>
+                  <c:v>8809</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3738</c:v>
+                  <c:v>4428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1053,7 +1054,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1175,7 +1175,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1275,7 +1274,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1409,7 +1407,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1417,6 +1414,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1653,34 +1651,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>1959512</c:v>
+                  <c:v>1959666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2569363</c:v>
+                  <c:v>2615715</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2323495</c:v>
+                  <c:v>2331477</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1981567</c:v>
+                  <c:v>1982634</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2177841</c:v>
+                  <c:v>2187411</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3086566</c:v>
+                  <c:v>3282060</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3508982</c:v>
+                  <c:v>3513194</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3633563</c:v>
+                  <c:v>3670798</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3222727</c:v>
+                  <c:v>3249657</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3246303</c:v>
+                  <c:v>3248009</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2700359</c:v>
@@ -1710,7 +1708,7 @@
                   <c:v>1973775</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2386392</c:v>
+                  <c:v>2388640</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>2739807</c:v>
@@ -1719,13 +1717,13 @@
                   <c:v>3432663</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3826308</c:v>
+                  <c:v>3827126</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3947312</c:v>
+                  <c:v>3947924</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1628710</c:v>
+                  <c:v>1941440</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1782,7 +1780,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1904,7 +1901,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1979,7 +1975,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1987,6 +1982,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3101,7 +3097,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="70" workbookViewId="0"/>
@@ -3113,7 +3109,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" workbookViewId="0"/>
@@ -3128,7 +3124,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8654143" cy="6272893"/>
+    <xdr:ext cx="8654143" cy="6277429"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3279,10 +3275,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8654143" cy="6272893"/>
+    <xdr:ext cx="8654143" cy="6277429"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
@@ -3408,7 +3410,7 @@
             <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0">
               <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Updated: May 20, 2025</a:t>
+            <a:t>Updated: May 26, 2025</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" kern="1200">
             <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
@@ -3736,16 +3738,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3759,147 +3761,147 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>94</v>
       </c>
       <c r="B2">
-        <v>4118</v>
+        <v>4119</v>
       </c>
       <c r="C2">
-        <v>1959512</v>
+        <v>1959666</v>
       </c>
       <c r="D2">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>95</v>
       </c>
       <c r="B3">
-        <v>5297</v>
+        <v>5403</v>
       </c>
       <c r="C3">
-        <v>2569363</v>
+        <v>2615715</v>
       </c>
       <c r="D3">
-        <v>621</v>
+        <v>633</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>96</v>
       </c>
       <c r="B4">
-        <v>4929</v>
+        <v>4948</v>
       </c>
       <c r="C4">
-        <v>2323495</v>
+        <v>2331477</v>
       </c>
       <c r="D4">
-        <v>608</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>97</v>
       </c>
       <c r="B5">
-        <v>4334</v>
+        <v>4339</v>
       </c>
       <c r="C5">
-        <v>1981567</v>
+        <v>1982634</v>
       </c>
       <c r="D5">
-        <v>469</v>
+        <v>473</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>98</v>
       </c>
       <c r="B6">
-        <v>4866</v>
+        <v>4889</v>
       </c>
       <c r="C6">
-        <v>2177841</v>
+        <v>2187411</v>
       </c>
       <c r="D6">
-        <v>616</v>
+        <v>623</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>99</v>
       </c>
       <c r="B7">
-        <v>6790</v>
+        <v>7205</v>
       </c>
       <c r="C7">
-        <v>3086566</v>
+        <v>3282060</v>
       </c>
       <c r="D7">
-        <v>654</v>
+        <v>666</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>100</v>
       </c>
       <c r="B8">
-        <v>7836</v>
+        <v>7851</v>
       </c>
       <c r="C8">
-        <v>3508982</v>
+        <v>3513194</v>
       </c>
       <c r="D8">
-        <v>702</v>
+        <v>713</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>101</v>
       </c>
       <c r="B9">
-        <v>8206</v>
+        <v>8287</v>
       </c>
       <c r="C9">
-        <v>3633563</v>
+        <v>3670798</v>
       </c>
       <c r="D9">
-        <v>640</v>
+        <v>650</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>102</v>
       </c>
       <c r="B10">
-        <v>7468</v>
+        <v>7540</v>
       </c>
       <c r="C10">
-        <v>3222727</v>
+        <v>3249657</v>
       </c>
       <c r="D10">
-        <v>578</v>
+        <v>590</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>103</v>
       </c>
       <c r="B11">
-        <v>7540</v>
+        <v>7547</v>
       </c>
       <c r="C11">
-        <v>3246303</v>
+        <v>3248009</v>
       </c>
       <c r="D11">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>104</v>
       </c>
@@ -3913,7 +3915,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>105</v>
       </c>
@@ -3927,7 +3929,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>106</v>
       </c>
@@ -3941,7 +3943,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>107</v>
       </c>
@@ -3955,7 +3957,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>108</v>
       </c>
@@ -3969,7 +3971,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>109</v>
       </c>
@@ -3983,7 +3985,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>110</v>
       </c>
@@ -3997,7 +3999,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>111</v>
       </c>
@@ -4011,7 +4013,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>112</v>
       </c>
@@ -4025,21 +4027,21 @@
         <v>283</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>113</v>
       </c>
       <c r="B21">
-        <v>5334</v>
+        <v>5342</v>
       </c>
       <c r="C21">
-        <v>2386392</v>
+        <v>2388640</v>
       </c>
       <c r="D21">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>114</v>
       </c>
@@ -4053,7 +4055,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>115</v>
       </c>
@@ -4067,60 +4069,46 @@
         <v>442</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>116</v>
       </c>
       <c r="B24">
-        <v>8498</v>
+        <v>8501</v>
       </c>
       <c r="C24">
-        <v>3826308</v>
+        <v>3827126</v>
       </c>
       <c r="D24">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>117</v>
       </c>
       <c r="B25">
-        <v>8806</v>
+        <v>8809</v>
       </c>
       <c r="C25">
-        <v>3947312</v>
+        <v>3947924</v>
       </c>
       <c r="D25">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>118</v>
       </c>
       <c r="B26">
-        <v>3738</v>
+        <v>4428</v>
       </c>
       <c r="C26">
-        <v>1628710</v>
+        <v>1941440</v>
       </c>
       <c r="D26">
         <v>274</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27">
-        <v>119</v>
-      </c>
-      <c r="B27">
-        <v>46</v>
-      </c>
-      <c r="C27">
-        <v>18842</v>
-      </c>
-      <c r="D27">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>